<commit_message>
se continua con las adecuaciones derivadas de cambios en tablas en cuanto a aumentar campos en ellas tales como unidad de medida etc
</commit_message>
<xml_diff>
--- a/ejemploinventarios.xlsx
+++ b/ejemploinventarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wampNuevo\www\matservices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MatservicesDeskGH\MatservicesD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>